<commit_message>
Handle toast on add new Account
</commit_message>
<xml_diff>
--- a/raw/New Accounts Data.xlsx
+++ b/raw/New Accounts Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farhanilhamdi/Katalon Studio/FinalMobileAutomationTest/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{312D96AD-36A6-CE43-98A1-95C436CF74D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36057FDE-0F2D-9C47-8E0C-67D54F578811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15820" xr2:uid="{736E790A-7B0E-B345-9B63-DDF8FB1BE8A9}"/>
   </bookViews>
@@ -402,7 +402,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -420,29 +420,30 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>